<commit_message>
slight updates added gerbers
</commit_message>
<xml_diff>
--- a/Raven/RX/MicroRX_RFM/MicroRX_RFM_BOM.xlsx
+++ b/Raven/RX/MicroRX_RFM/MicroRX_RFM_BOM.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Qty</t>
   </si>
@@ -199,9 +199,6 @@
     <t>JST 1MM Right angle 6pin male</t>
   </si>
   <si>
-    <t>LFCN-XXX (Mini-Circuits)</t>
-  </si>
-  <si>
     <t>RESISTOR_603</t>
   </si>
   <si>
@@ -215,13 +212,19 @@
   </si>
   <si>
     <t>MicroRX_RFM  Parts List</t>
+  </si>
+  <si>
+    <t>The difference between the 2 versions is the output filter. The rev0.1 uses the Johanson Technology 0500LP15A500E or 0900LP15B0063E</t>
+  </si>
+  <si>
+    <t>LFCN-490 (Mini-Circuits) for 433</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +234,13 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -257,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -265,14 +275,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E24"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,11 +608,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -647,13 +660,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>9</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>0.1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -696,7 +709,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
@@ -710,7 +723,7 @@
         <v>470</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
@@ -721,10 +734,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -775,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -796,10 +809,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -848,7 +861,7 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -910,9 +923,36 @@
         <v>34</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B27:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>